<commit_message>
Converted Excel Database from Cells to Tables
- To better integrate with the excel library, ClosedXML, the faux tables were made into real tables
</commit_message>
<xml_diff>
--- a/AirportExcels/AirportInfo.xlsx
+++ b/AirportExcels/AirportInfo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b8f136795524a28e/Documents/AirportExcels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dxvia\Documents\GitHub\EECS-3550-Team-2\AirportExcels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{830058BF-4106-4964-86E8-CFABB14438CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE60B23D-EA6F-481B-9AAC-7B1E654C6025}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAC4EF8-178C-4E58-9649-C94DC7F6FA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{3FBE4BD0-15DC-440E-AAB6-2D33A5BF3E36}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3FBE4BD0-15DC-440E-AAB6-2D33A5BF3E36}"/>
   </bookViews>
   <sheets>
     <sheet name="CustList" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Password</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Destination</t>
   </si>
   <si>
-    <t xml:space="preserve">From </t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -126,16 +123,25 @@
   </si>
   <si>
     <t>Total Capacity</t>
+  </si>
+  <si>
+    <t>From</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -180,8 +186,65 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1D1A64D8-5EAC-48C4-AA91-26DEBBFD94EB}" name="Table5" displayName="Table5" ref="A1:J3" totalsRowShown="0">
+  <autoFilter ref="A1:J3" xr:uid="{1D1A64D8-5EAC-48C4-AA91-26DEBBFD94EB}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{CC8B18D3-B80D-4944-A678-6AA2491E893B}" name="UserID"/>
+    <tableColumn id="2" xr3:uid="{8621CC71-A4AB-4F21-8532-B81F769DDBDA}" name="Password"/>
+    <tableColumn id="3" xr3:uid="{08739A7B-5B09-434E-BFF5-FD8318F1AA37}" name="FirstName"/>
+    <tableColumn id="4" xr3:uid="{9E077882-18CE-4DE1-BA37-CF4110DFE992}" name="LastName"/>
+    <tableColumn id="5" xr3:uid="{C7ADB1CA-8D50-4560-97FC-15989D8266E5}" name="Address"/>
+    <tableColumn id="6" xr3:uid="{8466F02A-F898-4E2C-B8EF-32517F3E7820}" name="Phone"/>
+    <tableColumn id="7" xr3:uid="{107480CD-39C0-43A0-8443-1F9D084DC1AA}" name="Age"/>
+    <tableColumn id="8" xr3:uid="{DB461F86-CEA7-4DF1-A8BD-8BA5B94B3506}" name="Wallet"/>
+    <tableColumn id="9" xr3:uid="{A10A9D0E-4802-4CD8-882D-42283D1BB655}" name="RewardPoints"/>
+    <tableColumn id="10" xr3:uid="{68D2C70A-1BA4-47D2-A119-5C8A5BECDE5E}" name="CardInfo"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EB54C36C-3D90-4A33-A0A7-C9DD68AC3F4B}" name="Table4" displayName="Table4" ref="A1:G3" totalsRowShown="0">
+  <autoFilter ref="A1:G3" xr:uid="{EB54C36C-3D90-4A33-A0A7-C9DD68AC3F4B}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{04C0CC16-FA33-471F-BF86-1AC94A19B138}" name="CustID"/>
+    <tableColumn id="2" xr3:uid="{78D16A40-1FC5-4306-8726-7D671101B344}" name="FlightID"/>
+    <tableColumn id="3" xr3:uid="{A5D8796A-1D39-4990-BE1C-8C1E2762947C}" name="Date"/>
+    <tableColumn id="4" xr3:uid="{C3C7D3D6-BC45-4339-8CB9-6D1F6C430874}" name="Status"/>
+    <tableColumn id="5" xr3:uid="{F14BD165-2B30-45C3-A902-05A758F9F30C}" name="From"/>
+    <tableColumn id="6" xr3:uid="{41AD29F5-0497-45CF-B9D9-CFFCB1633208}" name="Destination"/>
+    <tableColumn id="7" xr3:uid="{6F5FE047-F776-415E-9ED8-A734A4F7A628}" name="Points Used"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7D5E9CAD-81CA-46DB-89A6-8318481E2059}" name="Table3" displayName="Table3" ref="A1:D2" totalsRowShown="0">
+  <autoFilter ref="A1:D2" xr:uid="{7D5E9CAD-81CA-46DB-89A6-8318481E2059}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{CBAC46F9-7D88-464F-BB29-FADEF69E9A92}" name="EmpID"/>
+    <tableColumn id="2" xr3:uid="{D1ABA3E2-C682-4498-920F-7FE46A94B218}" name="Password"/>
+    <tableColumn id="3" xr3:uid="{9FA5A2AC-2509-4323-87B0-BE63F892C793}" name="FirstName"/>
+    <tableColumn id="4" xr3:uid="{3980335A-CF3C-41E5-96DF-AA28AB0F1AE7}" name="LastName"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C658C81C-7DED-4686-9739-ABD4A86EDD18}" name="Table2" displayName="Table2" ref="A1:D2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:D2" xr:uid="{C658C81C-7DED-4686-9739-ABD4A86EDD18}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C2A4DCF5-101B-4A91-A242-0FB4E17DCB7B}" name="FlightID"/>
+    <tableColumn id="2" xr3:uid="{1A7A2015-2474-4FDF-8FE6-66D4B55C9FD6}" name="Income"/>
+    <tableColumn id="3" xr3:uid="{20AE48E3-E9EE-4B79-B6D8-C26427168800}" name="Total Capacity"/>
+    <tableColumn id="4" xr3:uid="{9A1D826E-955D-4BD2-B808-B87A802CB4BD}" name="Booked Capacity"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -483,13 +546,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F89F44-A481-4375-B1EC-C94DE9571F7E}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8:X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="5" width="11" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -583,35 +648,43 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21FF9086-090E-4734-B9FF-8431E3318B82}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="L5" sqref="L5:R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
         <v>18</v>
@@ -620,18 +693,21 @@
         <v>17</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -640,14 +716,17 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C5"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -661,39 +740,65 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939E04D8-A099-4F29-89C5-2DBCE7E9A2F4}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" t="s">
         <v>27</v>
+      </c>
+      <c r="P7" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Preliminary Load engineer work
- Preliminary work getting a consistent excel grab
- Preliminary work on Load Engineer createFlight
- Minor class changes to Location, Flight, and Load Engineer instance variables
- Further commenting for clarity
- Installed ClosedXML
</commit_message>
<xml_diff>
--- a/AirportExcels/AirportInfo.xlsx
+++ b/AirportExcels/AirportInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dxvia\Documents\GitHub\EECS-3550-Team-2\AirportExcels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAC4EF8-178C-4E58-9649-C94DC7F6FA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EBB2E7-64B4-4A5C-9DA4-132D2227E7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3FBE4BD0-15DC-440E-AAB6-2D33A5BF3E36}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{3FBE4BD0-15DC-440E-AAB6-2D33A5BF3E36}"/>
   </bookViews>
   <sheets>
     <sheet name="CustList" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Password</t>
   </si>
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F89F44-A481-4375-B1EC-C94DE9571F7E}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8:X10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,10 +753,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939E04D8-A099-4F29-89C5-2DBCE7E9A2F4}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7:Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,7 +767,7 @@
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -778,20 +778,6 @@
         <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="M7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N7" t="s">
-        <v>25</v>
-      </c>
-      <c r="O7" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>